<commit_message>
Some test scripts added and some are modified
</commit_message>
<xml_diff>
--- a/com.crm.OrangeHRMENE/src/test/resources/OrangeHRMTestCases.xlsx
+++ b/com.crm.OrangeHRMENE/src/test/resources/OrangeHRMTestCases.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\com.crm.OrangeHRMENE\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB4F785-FF00-4091-A06E-874A05433053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A2CB5D-FF42-4D12-9FA3-8C68C95E455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6C101999-B80D-49C9-9EF7-1E10C2558C2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6C101999-B80D-49C9-9EF7-1E10C2558C2E}"/>
   </bookViews>
   <sheets>
     <sheet name=" Functional Testing" sheetId="1" r:id="rId1"/>
     <sheet name="LoginTestData" sheetId="4" r:id="rId2"/>
-    <sheet name="Integration testing" sheetId="2" r:id="rId3"/>
-    <sheet name="Compatibilty" sheetId="3" r:id="rId4"/>
+    <sheet name="AdminTestData" sheetId="5" r:id="rId3"/>
+    <sheet name="Integration testing" sheetId="2" r:id="rId4"/>
+    <sheet name="Compatibilty" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="1437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1441">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -4667,6 +4668,18 @@
   </si>
   <si>
     <t>'OR '1'='1</t>
+  </si>
+  <si>
+    <t>Roshan</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>Unnati</t>
+  </si>
+  <si>
+    <t>Dnyaneshwari</t>
   </si>
 </sst>
 </file>
@@ -11555,7 +11568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEA4FAD-2AC0-47E1-9B05-F7158B4DA1EB}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -11674,6 +11687,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9D74A5-8782-461A-A1F6-621954F4A4CA}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04AFB44-C52D-49C4-B945-4A693C6CB651}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -12426,7 +12487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7C5130-A8EC-4B1F-A647-800C40DD620A}">
   <dimension ref="A1:I31"/>
   <sheetViews>

</xml_diff>